<commit_message>
changed excel data set
</commit_message>
<xml_diff>
--- a/ProductDataSet.xlsx
+++ b/ProductDataSet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xpand\OneDrive - Xpand Solutions - Informática e Novas Tecnologias Lda\Power Platform\PowerGym\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\powerplatform-powergym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="11_B8DEAF55B0580082D603D7983459409E7F8F57BB" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6F8CEE88-5022-42A3-81C9-DF80FCFA3D18}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEEA938-0179-4C5E-BBCE-863EF492B8E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>ProductID</t>
   </si>
@@ -50,12 +50,6 @@
   </si>
   <si>
     <t>Characteristics</t>
-  </si>
-  <si>
-    <t>Documentation[image]</t>
-  </si>
-  <si>
-    <t>Photo[image]</t>
   </si>
   <si>
     <t>__PowerAppsId__</t>
@@ -81,15 +75,6 @@
 Analysis Fee - 252,80€</t>
   </si>
   <si>
-    <t>https://www.santandertotta.pt/pt_PT/pdf/BST-IE-500006775-FIN.jpg</t>
-  </si>
-  <si>
-    <t>https://www.rankia.pt/wp-content/uploads/2018/09/credito-habitacao.jpg</t>
-  </si>
-  <si>
-    <t>WFKA6ChIvP4</t>
-  </si>
-  <si>
     <t>Ever Growing Savings</t>
   </si>
   <si>
@@ -109,12 +94,6 @@
 Interest grows gradually</t>
   </si>
   <si>
-    <t>https://bancos.pt/wp-content/uploads/2015/11/deposito-millennium-770x310.jpg</t>
-  </si>
-  <si>
-    <t>VQYeAqo9R1U</t>
-  </si>
-  <si>
     <t>Revenue</t>
   </si>
   <si>
@@ -128,12 +107,6 @@
 Minimum Term Recommended: 6 months
 Risk Class: 2 - Low Risk
 Profitability: 0.93% (last 12 months)</t>
-  </si>
-  <si>
-    <t>http://www.forum-dinheiro.com/wp-content/uploads/2017/09/Vantagens-e-desvantagens-de-uma-Conta-Ordenado.jpg</t>
-  </si>
-  <si>
-    <t>oA5AL0RZOFc</t>
   </si>
   <si>
     <t>Net Deposit</t>
@@ -150,12 +123,6 @@
 Term - 31, 92, 183 or 366 days
 It doesn't allow reinforcements
 Interest is paid at the end of the term</t>
-  </si>
-  <si>
-    <t>https://www.contasconnosco.pt/storage/media/715/conversions/sao-estes-os-tres-melhores-depositos-a-prazo-em-2018-5a86bf6903112-large.jpg</t>
-  </si>
-  <si>
-    <t>TDfJjJbUsT0</t>
   </si>
   <si>
     <t>Ready Credit</t>
@@ -176,12 +143,6 @@
 Fixed interest rate</t>
   </si>
   <si>
-    <t>https://www.iq.com.br/wp-content/uploads/2018/06/emprestimo-pessoal.jpg</t>
-  </si>
-  <si>
-    <t>NKUJVQsySrY</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -192,6 +153,24 @@
   </si>
   <si>
     <t>7GvcffR1DnU</t>
+  </si>
+  <si>
+    <t>Photo</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/01_Mortgage%20Loan.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/02_EG%20Savings.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/03_Revenue_tn.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/04_Net%20Deposit.jpg</t>
+  </si>
+  <si>
+    <t>http://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/05_Ready%20Credit.jpg</t>
   </si>
 </sst>
 </file>
@@ -201,7 +180,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hyy\pe\r"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,11 +260,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
@@ -293,31 +269,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -331,18 +305,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Products" displayName="Products" ref="A1:I6" totalsRowShown="0">
-  <autoFilter ref="A1:I6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Products" displayName="Products" ref="A1:G6" totalsRowShown="0">
+  <autoFilter ref="A1:G6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ProductID"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Product Name"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ProductType"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Description"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Characteristics"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Documentation[image]"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Photo[image]"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="__PowerAppsId__"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Photo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -624,217 +596,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="37.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="28.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="120" customHeight="1">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="3" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" ht="120" customHeight="1">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="10"/>
-    </row>
-    <row r="4" spans="1:11" ht="120" customHeight="1">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="11" t="s">
+      <c r="F6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" ht="120" customHeight="1">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" spans="1:11" ht="120" customHeight="1">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="G6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="2"/>
+      <c r="H6" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H2" r:id="rId3" xr:uid="{4879157A-A7AC-4492-B40B-3865F45E4421}"/>
+    <hyperlink ref="G2" r:id="rId1" display="https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/01_Mortgage Loan.jpg" xr:uid="{FD57BC23-CA75-452B-9E5F-D74B60014D1A}"/>
+    <hyperlink ref="G3" r:id="rId2" display="https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/02_EG Savings.jpg" xr:uid="{D5FB3505-9ACE-4937-AA1F-BAEECEC060A8}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{5D91D2EE-DCA2-452A-A6E9-14CF57EEEF62}"/>
+    <hyperlink ref="G5" r:id="rId4" display="https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/04_Net Deposit.jpg" xr:uid="{85A0E91D-58A0-40EA-A603-7B73A7726A33}"/>
+    <hyperlink ref="G6" r:id="rId5" display="http://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/05_Ready Credit.jpg" xr:uid="{48D639EF-6ED6-480D-9B2F-30D5BE8DA845}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
@@ -847,38 +783,38 @@
       <selection activeCell="B2" sqref="B2 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="18.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="18.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="7" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="13">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>45</v>
+      <c r="D2" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Documentation column do excel product data set
</commit_message>
<xml_diff>
--- a/ProductDataSet.xlsx
+++ b/ProductDataSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\powerplatform-powergym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEEA938-0179-4C5E-BBCE-863EF492B8E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1262E4DD-48C7-4DFA-969F-5DACEDEB62EE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>ProductID</t>
   </si>
@@ -171,6 +171,24 @@
   </si>
   <si>
     <t>http://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/05_Ready%20Credit.jpg</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/01_FINE_Mortgage.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/03_Revenue.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/02_FIN DP Deposito Super Crescente_01082019.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/05_FDA CA Credito Pronto.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/04_FIN DP Net.pdf</t>
   </si>
 </sst>
 </file>
@@ -287,7 +305,18 @@
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -305,16 +334,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Products" displayName="Products" ref="A1:G6" totalsRowShown="0">
-  <autoFilter ref="A1:G6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Products" displayName="Products" ref="A1:H6" totalsRowShown="0">
+  <autoFilter ref="A1:H6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ProductID"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Product Name"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ProductType"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Description"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Characteristics"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Photo" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Photo" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{D94740E4-5394-4B40-9A1F-DF0D92B60B9C}" name="Documentation" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -599,7 +629,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,6 +641,7 @@
     <col min="5" max="5" width="37.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="33" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -635,7 +666,9 @@
       <c r="G1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
@@ -659,7 +692,9 @@
       <c r="G2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -683,7 +718,9 @@
       <c r="G3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -708,7 +745,9 @@
       <c r="G4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -732,7 +771,9 @@
       <c r="G5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -757,7 +798,9 @@
       <c r="G6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="10" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -766,11 +809,16 @@
     <hyperlink ref="G4" r:id="rId3" xr:uid="{5D91D2EE-DCA2-452A-A6E9-14CF57EEEF62}"/>
     <hyperlink ref="G5" r:id="rId4" display="https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/04_Net Deposit.jpg" xr:uid="{85A0E91D-58A0-40EA-A603-7B73A7726A33}"/>
     <hyperlink ref="G6" r:id="rId5" display="http://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/05_Ready Credit.jpg" xr:uid="{48D639EF-6ED6-480D-9B2F-30D5BE8DA845}"/>
+    <hyperlink ref="H2" r:id="rId6" xr:uid="{1007391A-E6A3-4AB0-9ECA-58E201B75A35}"/>
+    <hyperlink ref="H3" r:id="rId7" xr:uid="{51572EA2-B4A2-4797-9131-06D47C3D0F89}"/>
+    <hyperlink ref="H4" r:id="rId8" xr:uid="{EB831017-8A30-4595-8C64-FFEE1E812AEF}"/>
+    <hyperlink ref="H5" r:id="rId9" xr:uid="{3ACC8F4C-C2BB-4ED5-B7AC-D761302F90D8}"/>
+    <hyperlink ref="H6" r:id="rId10" xr:uid="{0ACFEAE3-54E8-4B79-B925-3CD97B944F5F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added new version of completed powerapp gym
</commit_message>
<xml_diff>
--- a/ProductDataSet.xlsx
+++ b/ProductDataSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\powerplatform-powergym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1262E4DD-48C7-4DFA-969F-5DACEDEB62EE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5F39BD-D61A-42D6-BD98-C7BAB3DB859C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>ProductID</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>Characteristics</t>
-  </si>
-  <si>
-    <t>__PowerAppsId__</t>
   </si>
   <si>
     <t>Mortgage Loan</t>
@@ -152,9 +149,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>7GvcffR1DnU</t>
-  </si>
-  <si>
     <t>Photo</t>
   </si>
   <si>
@@ -164,9 +158,6 @@
     <t>https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/02_EG%20Savings.jpg</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/03_Revenue_tn.jpg</t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/04_Net%20Deposit.jpg</t>
   </si>
   <si>
@@ -189,6 +180,9 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/04_FIN DP Net.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xpandit/powerplatform-powergym/master/Assets/03_Revenue.jpg</t>
   </si>
 </sst>
 </file>
@@ -351,13 +345,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Subscription" displayName="Subscription" ref="A1:D2" totalsRowShown="0">
-  <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Subscription" displayName="Subscription" ref="A1:C2" totalsRowShown="0">
+  <autoFilter ref="A1:C2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Product"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Full Name"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Email"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="__PowerAppsId__"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -628,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,10 +657,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -675,25 +668,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="G2" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -701,25 +694,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="G3" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I3" s="7"/>
     </row>
@@ -728,25 +721,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="G4" s="10" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -754,25 +747,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="G5" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I5" s="7"/>
     </row>
@@ -781,25 +774,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="G6" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -825,10 +818,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED5955F-2A91-447C-8B22-4D2DD58999CD}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2 B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,32 +830,26 @@
     <col min="2" max="3" width="18.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>